<commit_message>
Removed protection from spreadsheet so it works with Excel mobile. Made minor cosmetic changes
</commit_message>
<xml_diff>
--- a/KCCA Summer Quickplay results sheet.xlsx
+++ b/KCCA Summer Quickplay results sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\old data\old data\Users\Lenovo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{566F63F2-6834-4C10-83D1-A70ADE7DFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B714559-DCAB-4D69-8061-BC59A735EE11}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="13_ncr:1_{566F63F2-6834-4C10-83D1-A70ADE7DFAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47590780-B040-4B29-8E84-94CBD9732480}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>B1</t>
   </si>
   <si>
-    <t>HOME PLAYER 1</t>
+    <t xml:space="preserve">HOME PLAYER </t>
   </si>
   <si>
     <t>A2</t>
@@ -719,11 +719,48 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="12" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,45 +776,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1094,8 +1094,8 @@
   <dimension ref="B1:X56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1113,74 +1113,74 @@
     <col min="20" max="20" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="23.25" customHeight="1">
-      <c r="C1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="O1" s="39" t="s">
+    <row r="1" spans="2:24" ht="25.5">
+      <c r="C1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="O1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="39"/>
-    </row>
-    <row r="2" spans="2:24" ht="21" customHeight="1">
-      <c r="C2" s="49" t="s">
+      <c r="P1" s="40"/>
+    </row>
+    <row r="2" spans="2:24">
+      <c r="C2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="2:24" ht="24.95" customHeight="1">
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="45" t="s">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48" t="s">
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="2:24" ht="5.0999999999999996" customHeight="1"/>
     <row r="5" spans="2:24" ht="14.25" customHeight="1">
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="2:24">
       <c r="C6" s="22"/>
@@ -1231,10 +1231,10 @@
       <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="43"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="17">
         <v>1500</v>
       </c>
@@ -1247,11 +1247,11 @@
       <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="44" t="str">
+      <c r="J8" s="39" t="str">
         <f>J30</f>
         <v>AWAY PLAYER 2</v>
       </c>
-      <c r="K8" s="44"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="18">
         <f>L30</f>
         <v>1500</v>
@@ -1280,10 +1280,10 @@
       <c r="B9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="17">
         <v>1500</v>
       </c>
@@ -1296,11 +1296,11 @@
       <c r="I9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="44" t="str">
+      <c r="J9" s="39" t="str">
         <f>J29</f>
         <v>AWAY PLAYER 1</v>
       </c>
-      <c r="K9" s="44"/>
+      <c r="K9" s="39"/>
       <c r="L9" s="18">
         <f>L29</f>
         <v>1500</v>
@@ -1329,10 +1329,10 @@
       <c r="B10" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="43"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="17">
         <v>1500</v>
       </c>
@@ -1345,11 +1345,11 @@
       <c r="I10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="35" t="str">
+      <c r="J10" s="50" t="str">
         <f>J32</f>
         <v>AWAY PLAYER 4</v>
       </c>
-      <c r="K10" s="36"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="18">
         <f>L32</f>
         <v>1500</v>
@@ -1378,10 +1378,10 @@
       <c r="B11" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="17">
         <v>1500</v>
       </c>
@@ -1394,11 +1394,11 @@
       <c r="I11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="32" t="str">
+      <c r="J11" s="31" t="str">
         <f>J31</f>
         <v>AWAY PLAYER 3</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="31"/>
       <c r="L11" s="18">
         <f>L31</f>
         <v>1500</v>
@@ -1477,11 +1477,11 @@
         <f>B8</f>
         <v>B1</v>
       </c>
-      <c r="C15" s="44" t="str">
+      <c r="C15" s="39" t="str">
         <f>C8</f>
-        <v>HOME PLAYER 1</v>
-      </c>
-      <c r="D15" s="44"/>
+        <v xml:space="preserve">HOME PLAYER </v>
+      </c>
+      <c r="D15" s="39"/>
       <c r="E15" s="18">
         <f>E8</f>
         <v>1500</v>
@@ -1495,11 +1495,11 @@
       <c r="I15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="35" t="str">
+      <c r="J15" s="50" t="str">
         <f>J32</f>
         <v>AWAY PLAYER 4</v>
       </c>
-      <c r="K15" s="36"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="18">
         <f>L32</f>
         <v>1500</v>
@@ -1519,11 +1519,11 @@
         <f t="shared" ref="B16:C16" si="1">B9</f>
         <v>B2</v>
       </c>
-      <c r="C16" s="44" t="str">
+      <c r="C16" s="39" t="str">
         <f t="shared" si="1"/>
         <v>HOME PLAYER 2</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="39"/>
       <c r="E16" s="18">
         <f t="shared" ref="E16:E18" si="2">E9</f>
         <v>1500</v>
@@ -1537,11 +1537,11 @@
       <c r="I16" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="32" t="str">
+      <c r="J16" s="31" t="str">
         <f>J31</f>
         <v>AWAY PLAYER 3</v>
       </c>
-      <c r="K16" s="32"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="18">
         <f>L31</f>
         <v>1500</v>
@@ -1561,11 +1561,11 @@
         <f t="shared" ref="B17:C17" si="4">B10</f>
         <v>B3</v>
       </c>
-      <c r="C17" s="44" t="str">
+      <c r="C17" s="39" t="str">
         <f t="shared" si="4"/>
         <v>HOME PLAYER 3</v>
       </c>
-      <c r="D17" s="44"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="18">
         <f t="shared" si="2"/>
         <v>1500</v>
@@ -1579,11 +1579,11 @@
       <c r="I17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="44" t="str">
+      <c r="J17" s="39" t="str">
         <f>J30</f>
         <v>AWAY PLAYER 2</v>
       </c>
-      <c r="K17" s="44"/>
+      <c r="K17" s="39"/>
       <c r="L17" s="18">
         <f>L30</f>
         <v>1500</v>
@@ -1603,11 +1603,11 @@
         <f t="shared" ref="B18:C18" si="5">B11</f>
         <v>B4</v>
       </c>
-      <c r="C18" s="44" t="str">
+      <c r="C18" s="39" t="str">
         <f t="shared" si="5"/>
         <v>HOME PLAYER 4</v>
       </c>
-      <c r="D18" s="44"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="18">
         <f t="shared" si="2"/>
         <v>1500</v>
@@ -1621,11 +1621,11 @@
       <c r="I18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="44" t="str">
+      <c r="J18" s="39" t="str">
         <f>J29</f>
         <v>AWAY PLAYER 1</v>
       </c>
-      <c r="K18" s="44"/>
+      <c r="K18" s="39"/>
       <c r="L18" s="18">
         <f>L29</f>
         <v>1500</v>
@@ -1690,11 +1690,11 @@
         <f>B8</f>
         <v>B1</v>
       </c>
-      <c r="C22" s="44" t="str">
+      <c r="C22" s="39" t="str">
         <f>C8</f>
-        <v>HOME PLAYER 1</v>
-      </c>
-      <c r="D22" s="44"/>
+        <v xml:space="preserve">HOME PLAYER </v>
+      </c>
+      <c r="D22" s="39"/>
       <c r="E22" s="18">
         <f>E8</f>
         <v>1500</v>
@@ -1708,11 +1708,11 @@
       <c r="I22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J22" s="32" t="str">
+      <c r="J22" s="31" t="str">
         <f>J31</f>
         <v>AWAY PLAYER 3</v>
       </c>
-      <c r="K22" s="32"/>
+      <c r="K22" s="31"/>
       <c r="L22" s="18">
         <f>L31</f>
         <v>1500</v>
@@ -1732,11 +1732,11 @@
         <f t="shared" ref="B23:C23" si="6">B9</f>
         <v>B2</v>
       </c>
-      <c r="C23" s="44" t="str">
+      <c r="C23" s="39" t="str">
         <f t="shared" si="6"/>
         <v>HOME PLAYER 2</v>
       </c>
-      <c r="D23" s="44"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="18">
         <f t="shared" ref="E23:E25" si="7">E9</f>
         <v>1500</v>
@@ -1750,11 +1750,11 @@
       <c r="I23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="35" t="str">
+      <c r="J23" s="50" t="str">
         <f>J32</f>
         <v>AWAY PLAYER 4</v>
       </c>
-      <c r="K23" s="36"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="18">
         <f>L32</f>
         <v>1500</v>
@@ -1774,11 +1774,11 @@
         <f t="shared" ref="B24:C24" si="9">B10</f>
         <v>B3</v>
       </c>
-      <c r="C24" s="44" t="str">
+      <c r="C24" s="39" t="str">
         <f t="shared" si="9"/>
         <v>HOME PLAYER 3</v>
       </c>
-      <c r="D24" s="44"/>
+      <c r="D24" s="39"/>
       <c r="E24" s="18">
         <f t="shared" si="7"/>
         <v>1500</v>
@@ -1792,11 +1792,11 @@
       <c r="I24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="44" t="str">
+      <c r="J24" s="39" t="str">
         <f>J29</f>
         <v>AWAY PLAYER 1</v>
       </c>
-      <c r="K24" s="44"/>
+      <c r="K24" s="39"/>
       <c r="L24" s="18">
         <f>L29</f>
         <v>1500</v>
@@ -1816,11 +1816,11 @@
         <f t="shared" ref="B25:C25" si="10">B11</f>
         <v>B4</v>
       </c>
-      <c r="C25" s="44" t="str">
+      <c r="C25" s="39" t="str">
         <f t="shared" si="10"/>
         <v>HOME PLAYER 4</v>
       </c>
-      <c r="D25" s="44"/>
+      <c r="D25" s="39"/>
       <c r="E25" s="18">
         <f t="shared" si="7"/>
         <v>1500</v>
@@ -1834,11 +1834,11 @@
       <c r="I25" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="44" t="str">
+      <c r="J25" s="39" t="str">
         <f>J30</f>
         <v>AWAY PLAYER 2</v>
       </c>
-      <c r="K25" s="44"/>
+      <c r="K25" s="39"/>
       <c r="L25" s="18">
         <f>L30</f>
         <v>1500</v>
@@ -1903,11 +1903,11 @@
         <f>B8</f>
         <v>B1</v>
       </c>
-      <c r="C29" s="44" t="str">
+      <c r="C29" s="39" t="str">
         <f>C8</f>
-        <v>HOME PLAYER 1</v>
-      </c>
-      <c r="D29" s="44"/>
+        <v xml:space="preserve">HOME PLAYER </v>
+      </c>
+      <c r="D29" s="39"/>
       <c r="E29" s="18">
         <f>E8</f>
         <v>1500</v>
@@ -1921,10 +1921,10 @@
       <c r="I29" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="43" t="s">
+      <c r="J29" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="K29" s="43"/>
+      <c r="K29" s="34"/>
       <c r="L29" s="17">
         <v>1500</v>
       </c>
@@ -1943,11 +1943,11 @@
         <f t="shared" ref="B30:C30" si="11">B9</f>
         <v>B2</v>
       </c>
-      <c r="C30" s="44" t="str">
+      <c r="C30" s="39" t="str">
         <f t="shared" si="11"/>
         <v>HOME PLAYER 2</v>
       </c>
-      <c r="D30" s="44"/>
+      <c r="D30" s="39"/>
       <c r="E30" s="18">
         <f t="shared" ref="E30:E32" si="12">E9</f>
         <v>1500</v>
@@ -1961,10 +1961,10 @@
       <c r="I30" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="43" t="s">
+      <c r="J30" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="43"/>
+      <c r="K30" s="34"/>
       <c r="L30" s="17">
         <v>1500</v>
       </c>
@@ -1983,11 +1983,11 @@
         <f t="shared" ref="B31:C31" si="14">B10</f>
         <v>B3</v>
       </c>
-      <c r="C31" s="44" t="str">
+      <c r="C31" s="39" t="str">
         <f t="shared" si="14"/>
         <v>HOME PLAYER 3</v>
       </c>
-      <c r="D31" s="44"/>
+      <c r="D31" s="39"/>
       <c r="E31" s="18">
         <f t="shared" si="12"/>
         <v>1500</v>
@@ -2001,10 +2001,10 @@
       <c r="I31" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="31" t="s">
+      <c r="J31" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="31"/>
+      <c r="K31" s="32"/>
       <c r="L31" s="17">
         <v>1500</v>
       </c>
@@ -2023,11 +2023,11 @@
         <f t="shared" ref="B32:C32" si="15">B11</f>
         <v>B4</v>
       </c>
-      <c r="C32" s="44" t="str">
+      <c r="C32" s="39" t="str">
         <f t="shared" si="15"/>
         <v>HOME PLAYER 4</v>
       </c>
-      <c r="D32" s="44"/>
+      <c r="D32" s="39"/>
       <c r="E32" s="18">
         <f t="shared" si="12"/>
         <v>1500</v>
@@ -2041,10 +2041,10 @@
       <c r="I32" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="37" t="s">
+      <c r="J32" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="K32" s="38"/>
+      <c r="K32" s="53"/>
       <c r="L32" s="17">
         <v>1500</v>
       </c>
@@ -2087,19 +2087,19 @@
     </row>
     <row r="36" spans="4:14" ht="20.25" customHeight="1"/>
     <row r="37" spans="4:14">
-      <c r="D37" s="51" t="s">
+      <c r="D37" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="53" t="s">
+      <c r="E37" s="36"/>
+      <c r="F37" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G37" s="53"/>
+      <c r="G37" s="37"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="53" t="s">
+      <c r="I37" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="54"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" spans="4:14">
       <c r="D38" s="4" t="s">
@@ -2337,49 +2337,48 @@
       </c>
     </row>
     <row r="55" spans="2:18" ht="14.25" customHeight="1">
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="50"/>
-      <c r="N55" s="50"/>
-      <c r="O55" s="50"/>
-      <c r="P55" s="50"/>
-      <c r="Q55" s="50"/>
-      <c r="R55" s="50"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="54"/>
+      <c r="I55" s="54"/>
+      <c r="J55" s="54"/>
+      <c r="K55" s="54"/>
+      <c r="L55" s="54"/>
+      <c r="M55" s="54"/>
+      <c r="N55" s="54"/>
+      <c r="O55" s="54"/>
+      <c r="P55" s="54"/>
+      <c r="Q55" s="54"/>
+      <c r="R55" s="54"/>
     </row>
     <row r="56" spans="2:18">
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="34"/>
-      <c r="P56" s="34"/>
-      <c r="Q56" s="34"/>
-      <c r="R56" s="34"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="49"/>
+      <c r="O56" s="49"/>
+      <c r="P56" s="49"/>
+      <c r="Q56" s="49"/>
+      <c r="R56" s="49"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="C3:F3" name="Home team name"/>
     <protectedRange sqref="J3:M3" name="Away team name"/>
@@ -2391,31 +2390,6 @@
     <protectedRange sqref="G8:G11 G15:G18 G22:G25 G29:G32 N29:N32 N22:N25 N15:N18 N8:N11" name="Player results"/>
   </protectedRanges>
   <mergeCells count="41">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="C5:M5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="J2:M2"/>
     <mergeCell ref="B56:R56"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J15:K15"/>
@@ -2432,6 +2406,31 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="B55:R55"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter home team name" sqref="C3:F3" xr:uid="{22094883-E645-4B7F-BDB7-0B2DB002B898}"/>

</xml_diff>